<commit_message>
migration to schema markup
</commit_message>
<xml_diff>
--- a/downloads/SIBP Exec Assessment 250203.xlsx
+++ b/downloads/SIBP Exec Assessment 250203.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/39cad19df2e8f612/SIBP/1 Practice Development/2 Exec Assessment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{F706B2E2-674F-6245-8DE2-92E8046F30C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93C9242A-3B42-3B4A-ACD9-6797B4F827AF}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{F706B2E2-674F-6245-8DE2-92E8046F30C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1AB5C28-76B2-5141-A447-4D3D8B266319}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Z5g3pkipscaoOdEwqiz2avhYcn2viAwWA5KHG/cNtldJJgUvw9+OkaV3xXFEAoIhuXbC4AbWZHa4OGIk3+j1KA==" workbookSaltValue="T+/Q59o/vN0yyCeE4qjwNQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="-14380" windowWidth="24340" windowHeight="14380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6720" yWindow="-15220" windowWidth="20460" windowHeight="15220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTIONS" sheetId="4" r:id="rId1"/>
@@ -628,6 +628,9 @@
   </si>
   <si>
     <t>For follow-up and to receive any updates from us, please provide the following details, and email this spreadsheet to the above contact.</t>
+  </si>
+  <si>
+    <t>If you have any questions or need further assistance while completing the questionnaire, please reach out to belliott@tompkinsventures.com .</t>
   </si>
   <si>
     <t>Once the Questionnaire has been completed, the summary of recommendations are presented below…</t>
@@ -747,15 +750,12 @@
   <si>
     <t>Are financial, operational, and supply chain plans integrated into a unified financial strategy?</t>
   </si>
-  <si>
-    <t>If you have any questions or need further assistance while completing the questionnaire, please reach out to info@sustainable-ibp.com</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -929,22 +929,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="14"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -1019,7 +1003,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1194,39 +1178,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1373,6 +1330,12 @@
     <xf numFmtId="0" fontId="23" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1384,12 +1347,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1440,15 +1397,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+  <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2144,10 +2094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B6EA3A-E482-B148-B299-652B50AB0846}">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2158,15 +2108,15 @@
   <sheetData>
     <row r="1" spans="1:2" s="14" customFormat="1" ht="218" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="45" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B1" s="45"/>
     </row>
     <row r="2" spans="1:2" s="14" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="54" t="s">
-        <v>203</v>
-      </c>
-      <c r="B2" s="55"/>
+      <c r="A2" s="56" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="57"/>
     </row>
     <row r="3" spans="1:2" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
@@ -2210,7 +2160,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="58" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="35" t="s">
         <v>185</v>
       </c>
@@ -2355,10 +2305,10 @@
       <c r="B29" s="51"/>
     </row>
     <row r="30" spans="1:2" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="75" t="s">
-        <v>224</v>
-      </c>
-      <c r="B30" s="76"/>
+      <c r="A30" s="52" t="s">
+        <v>197</v>
+      </c>
+      <c r="B30" s="53"/>
     </row>
     <row r="31" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="50" t="s">
@@ -2367,55 +2317,51 @@
       <c r="B31" s="51"/>
     </row>
     <row r="32" spans="1:2" s="12" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="52" t="s">
+      <c r="A32" s="54" t="s">
         <v>196</v>
       </c>
-      <c r="B32" s="53"/>
+      <c r="B32" s="55"/>
     </row>
     <row r="33" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="41" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B33" s="29"/>
     </row>
     <row r="34" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="41" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B34" s="30"/>
     </row>
     <row r="35" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="41" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B35" s="30"/>
     </row>
     <row r="36" spans="1:2" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A36" s="42" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B36" s="31"/>
     </row>
-    <row r="37" spans="1:2" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="56"/>
-      <c r="B37" s="57"/>
-    </row>
-    <row r="38" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="50" t="s">
+    <row r="37" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="50" t="s">
         <v>126</v>
       </c>
-      <c r="B38" s="51"/>
-    </row>
-    <row r="39" spans="1:2" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="43" t="s">
+      <c r="B37" s="51"/>
+    </row>
+    <row r="38" spans="1:2" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="B39" s="44"/>
+      <c r="B38" s="44"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="zjjr3p+UK6SmXXaSNDTCCJnaNk0lCoB4OeSZMU8X3+NfUicOIrPqtbjpw8thSwlpATnwcTrHZywbdiRKzaYtTA==" saltValue="lNWdzoS+4mV/QgtYPqoxZg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="16">
-    <mergeCell ref="A39:B39"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="oXyjFpO5zuAXgq0WU87wlR9DiCM6D3CETnt1e47KZ01sk46dxsXoHsav1l0/HR0ZMwu63qJbzbLyx7B2HLvKKg==" saltValue="TTmRWWkOA5s7gZlPvacOcg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="15">
+    <mergeCell ref="A38:B38"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A7:B7"/>
@@ -2428,13 +2374,9 @@
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A37:B37"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A37:B37"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A30:B30" r:id="rId1" display="If you have any questions or need further assistance while completing the questionnaire, please reach out to info@sustainable-ibp.com" xr:uid="{D4DA46BE-CB0E-9140-907C-B536E03B9D13}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -2447,14 +2389,14 @@
   </sheetPr>
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.83203125" customWidth="1"/>
-    <col min="2" max="2" width="170.6640625" customWidth="1"/>
+    <col min="2" max="2" width="200.83203125" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2491,7 +2433,7 @@
       </c>
       <c r="C4" s="28"/>
     </row>
-    <row r="5" spans="1:4" ht="130" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16"/>
       <c r="B5" s="58" t="str">
         <f>KB!L5</f>
@@ -2509,7 +2451,7 @@
       </c>
       <c r="C6" s="28"/>
     </row>
-    <row r="7" spans="1:4" ht="130" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="100" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" s="60" t="str">
         <f>KB!L7</f>
@@ -2536,7 +2478,7 @@
       <c r="C9" s="28"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="130" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16"/>
       <c r="B10" s="58" t="str">
         <f>KB!L10</f>
@@ -2555,7 +2497,7 @@
       <c r="C11" s="28"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="130" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="100" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="60" t="str">
         <f>KB!L12</f>
@@ -2582,7 +2524,7 @@
       <c r="C14" s="28"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="130" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16"/>
       <c r="B15" s="58" t="str">
         <f>KB!L15</f>
@@ -2601,7 +2543,7 @@
       <c r="C16" s="28"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:3" ht="130" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="100" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="60" t="str">
         <f>KB!L17</f>
@@ -2626,7 +2568,7 @@
       </c>
       <c r="C19" s="28"/>
     </row>
-    <row r="20" spans="1:3" ht="130" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="16"/>
       <c r="B20" s="58" t="str">
         <f>KB!L20</f>
@@ -2644,7 +2586,7 @@
       </c>
       <c r="C21" s="28"/>
     </row>
-    <row r="22" spans="1:3" ht="130" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="100" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
       <c r="B22" s="60" t="str">
         <f>KB!L22</f>
@@ -2669,7 +2611,7 @@
       </c>
       <c r="C24" s="28"/>
     </row>
-    <row r="25" spans="1:3" ht="130" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="16"/>
       <c r="B25" s="58" t="str">
         <f>KB!L25</f>
@@ -2687,7 +2629,7 @@
       </c>
       <c r="C26" s="28"/>
     </row>
-    <row r="27" spans="1:3" ht="130" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="100" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="60" t="str">
         <f>KB!L27</f>
@@ -2712,7 +2654,7 @@
       </c>
       <c r="C29" s="28"/>
     </row>
-    <row r="30" spans="1:3" ht="130" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="16"/>
       <c r="B30" s="58" t="str">
         <f>KB!L30</f>
@@ -2730,7 +2672,7 @@
       </c>
       <c r="C31" s="28"/>
     </row>
-    <row r="32" spans="1:3" ht="130" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="100" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18"/>
       <c r="B32" s="60" t="str">
         <f>KB!L32</f>
@@ -2755,7 +2697,7 @@
       </c>
       <c r="C34" s="28"/>
     </row>
-    <row r="35" spans="1:3" ht="130" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="16"/>
       <c r="B35" s="58" t="str">
         <f>KB!L35</f>
@@ -2773,7 +2715,7 @@
       </c>
       <c r="C36" s="28"/>
     </row>
-    <row r="37" spans="1:3" ht="130" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="100" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="18"/>
       <c r="B37" s="60" t="str">
         <f>KB!L37</f>
@@ -2783,7 +2725,7 @@
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="19" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B38" s="25"/>
       <c r="C38" s="26"/>
@@ -2798,7 +2740,7 @@
       </c>
       <c r="C39" s="28"/>
     </row>
-    <row r="40" spans="1:3" ht="130" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="16"/>
       <c r="B40" s="58" t="str">
         <f>KB!L40</f>
@@ -2816,7 +2758,7 @@
       </c>
       <c r="C41" s="28"/>
     </row>
-    <row r="42" spans="1:3" ht="130" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="100" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18"/>
       <c r="B42" s="60" t="str">
         <f>KB!L42</f>
@@ -2825,19 +2767,8 @@
       <c r="C42" s="61"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="dfIBo2H/1zvX+5P3DNGbEQ3J2Oas0VWK62eYdjzj0wWnS0p6YRcyO82e/Dz6hS8lVhkQXN+RN8eikXZxUKdaWQ==" saltValue="pGswg4Zbm9VRy5IyRV5YvA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="SBN1JzXdFLJDN5kQ6su7Nd1MoKK2zQMI0HX07zxzhlQoQ/8Xzivw6OKnvB3NAWWmllcVJGqcFwZdBZm6c3nQYw==" saltValue="W0yE+3/tit/kssJe8v7H5w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B12:C12"/>
@@ -2845,6 +2776,17 @@
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B22:C22"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B37:C37"/>
   </mergeCells>
   <conditionalFormatting sqref="C4">
     <cfRule type="expression" dxfId="47" priority="60" stopIfTrue="1">
@@ -3048,7 +2990,7 @@
   <sheetData>
     <row r="2" spans="2:4" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
@@ -4400,7 +4342,7 @@
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="4"/>
       <c r="B39" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
@@ -4425,31 +4367,31 @@
         <v>8.1</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="K40" s="7">
         <f>_xlfn.SWITCH(QUESTIONNAIRE!C39,"",0,"NO",1,"UNSURE",2,"YES",3,0)</f>
@@ -4502,31 +4444,31 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="J42" s="8" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K42" s="7">
         <f>_xlfn.SWITCH(QUESTIONNAIRE!C41,"",0,"NO",1,"UNSURE",2,"YES",3,0)</f>
@@ -4795,7 +4737,7 @@
     <row r="57" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B57" s="10"/>
       <c r="L57" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="M57" s="7">
         <f>K39</f>

</xml_diff>